<commit_message>
Se agrego validacion nombre plan de estudio
</commit_message>
<xml_diff>
--- a/target/sistemaUniversidades_XP-1.0-SNAPSHOT/recursos/plantilla_importar_alumnos.xlsx
+++ b/target/sistemaUniversidades_XP-1.0-SNAPSHOT/recursos/plantilla_importar_alumnos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\NetBeansProjects\sistemaUniversidades_XP\src\main\webapp\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hector\Desktop\GIT\sistemaUniversidades_XP\src\main\webapp\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A165A882-6690-4EAD-B374-5E4B85CCAAA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="975" windowWidth="15375" windowHeight="9615" xr2:uid="{B2DADF52-93B2-4522-AF0D-E1CCEB769197}"/>
+    <workbookView xWindow="3255" yWindow="975" windowWidth="15375" windowHeight="9615"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,22 +24,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>101010</t>
-  </si>
-  <si>
-    <t>Ejemplo</t>
-  </si>
-  <si>
-    <t>CURPEJEMPLO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>PLAN ESTUDIO</t>
+  </si>
+  <si>
+    <t>MATRICULA</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>CURP</t>
+  </si>
+  <si>
+    <t>206275</t>
+  </si>
+  <si>
+    <t>LUIS ALEJANDRO</t>
+  </si>
+  <si>
+    <t>FEVC000117HSRLLRA5</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +64,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,10 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,30 +417,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B94E487-192F-4D1A-9784-D09C13C9DA62}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
     </row>
   </sheetData>

</xml_diff>